<commit_message>
new classification metrics tested
</commit_message>
<xml_diff>
--- a/tests/test_supervised/test_data/test_classification_metrics.xlsx
+++ b/tests/test_supervised/test_data/test_classification_metrics.xlsx
@@ -5,18 +5,57 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\Data Science\Projects\MLStudio\tests\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\Data Science\Projects\MLStudio\tests\test_supervised\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38370" windowHeight="4560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38370" windowHeight="4560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="metrics" sheetId="2" r:id="rId2"/>
+    <sheet name="worksheet" sheetId="2" r:id="rId2"/>
+    <sheet name="metrics" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$B$101</definedName>
+    <definedName name="ACC">worksheet!$P$2</definedName>
+    <definedName name="BACC">worksheet!$AA$2</definedName>
+    <definedName name="CK">worksheet!$AH$2</definedName>
+    <definedName name="CKC">worksheet!$AG$2</definedName>
+    <definedName name="CRR">worksheet!$R$2</definedName>
+    <definedName name="DR">worksheet!$Q$2</definedName>
+    <definedName name="F05_">worksheet!$AF$2</definedName>
+    <definedName name="F1_">worksheet!$AD$2</definedName>
+    <definedName name="F2_">worksheet!$AE$2</definedName>
+    <definedName name="FC">worksheet!$G$2</definedName>
+    <definedName name="FDR">worksheet!$T$2</definedName>
+    <definedName name="FN">worksheet!$D$2</definedName>
+    <definedName name="FNR">worksheet!$M$2</definedName>
+    <definedName name="FOR">worksheet!$U$2</definedName>
+    <definedName name="FP">worksheet!$C$2</definedName>
+    <definedName name="FPR">worksheet!$O$2</definedName>
+    <definedName name="GM">worksheet!$AB$2</definedName>
+    <definedName name="INFORM">worksheet!$Z$2</definedName>
+    <definedName name="LRN">worksheet!$Y$2</definedName>
+    <definedName name="LRP">worksheet!$X$2</definedName>
+    <definedName name="MARK">worksheet!$AC$2</definedName>
+    <definedName name="MCC">worksheet!$AI$2</definedName>
+    <definedName name="MCR">worksheet!$W$2</definedName>
+    <definedName name="N">worksheet!$K$2</definedName>
+    <definedName name="NPV">worksheet!$V$2</definedName>
+    <definedName name="ON">worksheet!$I$2</definedName>
+    <definedName name="OP">worksheet!$H$2</definedName>
+    <definedName name="OR">worksheet!$AJ$2</definedName>
+    <definedName name="P">worksheet!$J$2</definedName>
+    <definedName name="PPV">worksheet!$S$2</definedName>
+    <definedName name="PREV">worksheet!$AL$2</definedName>
+    <definedName name="SKEW">worksheet!$AM$2</definedName>
+    <definedName name="Sn">worksheet!$A$2</definedName>
+    <definedName name="TC">worksheet!$F$2</definedName>
+    <definedName name="TN">worksheet!$E$2</definedName>
+    <definedName name="TNR">worksheet!$N$2</definedName>
+    <definedName name="TP">worksheet!$B$2</definedName>
+    <definedName name="TPR">worksheet!$L$2</definedName>
     <definedName name="y">data!$A$2:$A$101</definedName>
     <definedName name="y_pred">data!$B$2:$B$101</definedName>
   </definedNames>
@@ -30,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
   <si>
     <t>y</t>
   </si>
@@ -38,31 +77,127 @@
     <t>y_pred</t>
   </si>
   <si>
-    <t>tp</t>
-  </si>
-  <si>
-    <t>fp</t>
-  </si>
-  <si>
-    <t>fn</t>
-  </si>
-  <si>
-    <t>tn</t>
-  </si>
-  <si>
-    <t>precision</t>
-  </si>
-  <si>
-    <t>recall</t>
-  </si>
-  <si>
-    <t>specificity</t>
-  </si>
-  <si>
-    <t>f1</t>
-  </si>
-  <si>
-    <t>ba</t>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>Sn</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TPR</t>
+  </si>
+  <si>
+    <t>FNR</t>
+  </si>
+  <si>
+    <t>TNR</t>
+  </si>
+  <si>
+    <t>FPR</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>CRR</t>
+  </si>
+  <si>
+    <t>PPV</t>
+  </si>
+  <si>
+    <t>FDR</t>
+  </si>
+  <si>
+    <t>FOR</t>
+  </si>
+  <si>
+    <t>NPV</t>
+  </si>
+  <si>
+    <t>MCR</t>
+  </si>
+  <si>
+    <t>LRP</t>
+  </si>
+  <si>
+    <t>LRN</t>
+  </si>
+  <si>
+    <t>INFORM</t>
+  </si>
+  <si>
+    <t>BACC</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>MARK</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F05</t>
+  </si>
+  <si>
+    <t>CK</t>
+  </si>
+  <si>
+    <t>CKC</t>
+  </si>
+  <si>
+    <t>MCC</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>PREV</t>
+  </si>
+  <si>
+    <t>SKEW</t>
+  </si>
+  <si>
+    <t>METRIC</t>
+  </si>
+  <si>
+    <t>VALUE</t>
   </si>
 </sst>
 </file>
@@ -382,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,17 +1338,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:AM21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -1228,54 +1363,651 @@
         <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2">
+        <f>COUNT(y)</f>
+        <v>100</v>
+      </c>
+      <c r="B2">
         <f>COUNTIFS(y,1,y_pred,1)</f>
         <v>27</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <f>COUNTIFS(y,0,y_pred,1)</f>
         <v>31</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <f>COUNTIFS(y,1,y_pred,0)</f>
         <v>20</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <f>COUNTIFS(y,0,y_pred,0)</f>
         <v>22</v>
       </c>
-      <c r="E2">
-        <f>A2/(A2+B2)</f>
+      <c r="F2">
+        <f>TP+TN</f>
+        <v>49</v>
+      </c>
+      <c r="G2">
+        <f>FP+FN</f>
+        <v>51</v>
+      </c>
+      <c r="H2">
+        <f>TP+FP</f>
+        <v>58</v>
+      </c>
+      <c r="I2">
+        <f>FN+TN</f>
+        <v>42</v>
+      </c>
+      <c r="J2">
+        <f>TP+FN</f>
+        <v>47</v>
+      </c>
+      <c r="K2">
+        <f>FP+TN</f>
+        <v>53</v>
+      </c>
+      <c r="L2">
+        <f>TP/P</f>
+        <v>0.57446808510638303</v>
+      </c>
+      <c r="M2">
+        <f>FN/P</f>
+        <v>0.42553191489361702</v>
+      </c>
+      <c r="N2">
+        <f>TN/N</f>
+        <v>0.41509433962264153</v>
+      </c>
+      <c r="O2">
+        <f>FP/N</f>
+        <v>0.58490566037735847</v>
+      </c>
+      <c r="P2">
+        <f>TC/Sn</f>
+        <v>0.49</v>
+      </c>
+      <c r="Q2">
+        <f>TP/Sn</f>
+        <v>0.27</v>
+      </c>
+      <c r="R2">
+        <f>TN/Sn</f>
+        <v>0.22</v>
+      </c>
+      <c r="S2">
+        <f>TP/OP</f>
         <v>0.46551724137931033</v>
       </c>
-      <c r="F2">
-        <f>A2/(A2+C2)</f>
+      <c r="T2">
+        <f>FP/OP</f>
+        <v>0.53448275862068961</v>
+      </c>
+      <c r="U2">
+        <f>FN/ON</f>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="V2">
+        <f>TN/ON</f>
+        <v>0.52380952380952384</v>
+      </c>
+      <c r="W2">
+        <f>FC/Sn</f>
+        <v>0.51</v>
+      </c>
+      <c r="X2">
+        <f>TPR/FPR</f>
+        <v>0.98215511324639682</v>
+      </c>
+      <c r="Y2">
+        <f>FNR/TNR</f>
+        <v>1.0251450676982592</v>
+      </c>
+      <c r="Z2">
+        <f>TPR+TNR-1</f>
+        <v>-1.0437575270975441E-2</v>
+      </c>
+      <c r="AA2">
+        <f>(TPR+TNR)/2</f>
+        <v>0.49478121236451228</v>
+      </c>
+      <c r="AB2">
+        <f>SQRT(TPR*TNR)</f>
+        <v>0.48832207652482545</v>
+      </c>
+      <c r="AC2">
+        <f>PPV+NPV-1</f>
+        <v>-1.0673234811165777E-2</v>
+      </c>
+      <c r="AD2">
+        <f>(2*PPV*TPR)/(PPV+TPR)</f>
+        <v>0.51428571428571435</v>
+      </c>
+      <c r="AE2">
+        <f>(5*PPV*TPR)/(4*PPV+TPR)</f>
+        <v>0.54878048780487809</v>
+      </c>
+      <c r="AF2">
+        <f>(1.25*PPV*TPR)/(0.25*PPV+TPR)</f>
+        <v>0.48387096774193544</v>
+      </c>
+      <c r="AG2">
+        <f>((P*OP)+(N*ON))/Sn^2</f>
+        <v>0.49519999999999997</v>
+      </c>
+      <c r="AH2">
+        <f>(ACC-CKC)/(1-CKC)</f>
+        <v>-1.0301109350237682E-2</v>
+      </c>
+      <c r="AI2">
+        <f>SQRT(INFORM*MARK)</f>
+        <v>1.0554747354926983E-2</v>
+      </c>
+      <c r="AJ2">
+        <f>(TP-TN)/(FP-FN)</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="AK2">
+        <f>SQRT(3)/PI()*LN(AJ2)</f>
+        <v>-0.43469932557681495</v>
+      </c>
+      <c r="AL2">
+        <f>P/Sn</f>
+        <v>0.47</v>
+      </c>
+      <c r="AM2">
+        <f>N/P</f>
+        <v>1.1276595744680851</v>
+      </c>
+    </row>
+    <row r="20" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="22:23" x14ac:dyDescent="0.25">
+      <c r="V21">
+        <v>2</v>
+      </c>
+      <c r="W21">
+        <f>V21+V20</f>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <f>COUNT(y)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f>COUNTIFS(y,1,y_pred,1)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIFS(y,0,y_pred,1)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <f>COUNTIFS(y,1,y_pred,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>COUNTIFS(y,0,y_pred,0)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <f>TP+TN</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <f>FP+FN</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <f>TP+FP</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <f>FN+TN</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <f>TP+FN</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <f>FP+TN</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <f>TP/P</f>
         <v>0.57446808510638303</v>
       </c>
-      <c r="G2">
-        <f>D2/(D2+B2)</f>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <f>FN/P</f>
+        <v>0.42553191489361702</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <f>TN/N</f>
         <v>0.41509433962264153</v>
       </c>
-      <c r="H2">
-        <f>2*A2/(2*A2+B2+C2)</f>
-        <v>0.51428571428571423</v>
-      </c>
-      <c r="I2">
-        <f>(F2+G2)/2</f>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <f>FP/N</f>
+        <v>0.58490566037735847</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <f>TC/Sn</f>
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <f>TP/Sn</f>
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <f>TN/Sn</f>
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <f>TP/OP</f>
+        <v>0.46551724137931033</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <f>FP/OP</f>
+        <v>0.53448275862068961</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <f>FN/ON</f>
+        <v>0.47619047619047616</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <f>TN/ON</f>
+        <v>0.52380952380952384</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <f>FC/Sn</f>
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <f>TPR/FPR</f>
+        <v>0.98215511324639682</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <f>FNR/TNR</f>
+        <v>1.0251450676982592</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <f>TPR+TNR-1</f>
+        <v>-1.0437575270975441E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28">
+        <f>(TPR+TNR)/2</f>
         <v>0.49478121236451228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <f>SQRT(TPR*TNR)</f>
+        <v>0.48832207652482545</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <f>PPV+NPV-1</f>
+        <v>-1.0673234811165777E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <f>(2*PPV*TPR)/(PPV+TPR)</f>
+        <v>0.51428571428571435</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <f>(5*PPV*TPR)/(4*PPV+TPR)</f>
+        <v>0.54878048780487809</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <f>(1.25*PPV*TPR)/(0.25*PPV+TPR)</f>
+        <v>0.48387096774193544</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34">
+        <f>((P*OP)+(N*ON))/Sn^2</f>
+        <v>0.49519999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <f>(ACC-CKC)/(1-CKC)</f>
+        <v>-1.0301109350237682E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <f>SQRT(INFORM*MARK)</f>
+        <v>1.0554747354926983E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <f>(TP-TN)/(FP-FN)</f>
+        <v>0.45454545454545453</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>-0.43469932557681495</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <f>P/Sn</f>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <f>N/P</f>
+        <v>1.1276595744680851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>